<commit_message>
created presentation and added burndown chart
</commit_message>
<xml_diff>
--- a/burndown chart/burndown.xlsx
+++ b/burndown chart/burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Studium\8.Semester\seminar\csseminar\burndown chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B18272-E9E1-4FDC-B04E-43C18F4719E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98868971-FCED-4DDB-84AE-E63F8988E634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1757,40 +1757,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2384,7 +2384,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2512,7 +2512,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="13">
         <f t="shared" ref="E3:E34" si="1">IF(D3&gt;C3,$D3-(SUM($G3:$W3)),$C3-(SUM($G3:$W3)))</f>
@@ -2545,7 +2545,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="1"/>
@@ -2628,7 +2628,7 @@
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="12">
-        <f t="shared" ref="D3:D34" si="2">IF(C8&lt;SUM(G8:W8),SUM(G8:W8),C8)</f>
+        <f t="shared" ref="D8:D34" si="2">IF(C8&lt;SUM(G8:W8),SUM(G8:W8),C8)</f>
         <v>0</v>
       </c>
       <c r="E8" s="13">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="D35" s="28">
         <f>SUM(D3:D34)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="E35" s="28">
         <f>SUM(E3:E34)</f>
@@ -3259,51 +3259,51 @@
       </c>
       <c r="F38" s="39">
         <f>D35</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="G38" s="39">
         <f>$D$35-SUM(G$3:G$34)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="H38" s="39">
         <f t="shared" ref="H38:Q38" si="5">G38-SUM(H3:H34)</f>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="I38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="J38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="K38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="L38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="M38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="N38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="O38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="P38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="Q38" s="39">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="R38" s="39"/>
       <c r="S38" s="39"/>
@@ -3986,7 +3986,7 @@
         <v>Submit and wait for grading</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>IF(ISBLANK(Chart!A7),"",Chart!A7)</f>
         <v>Writing Assignment 2: Background &amp; Related Work</v>

</xml_diff>

<commit_message>
updated burndown_chart and created outline
</commit_message>
<xml_diff>
--- a/burndown chart/burndown.xlsx
+++ b/burndown chart/burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Studium\8.Semester\seminar\csseminar\burndown chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98868971-FCED-4DDB-84AE-E63F8988E634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6778D825-C716-4AA9-B786-A336623AD84E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,10 +102,10 @@
     <t>Writing Assignment 2: Background &amp; Related Work</t>
   </si>
   <si>
-    <t>Writing Assignment 1: Proposal</t>
+    <t>Practice presentation</t>
   </si>
   <si>
-    <t>Practice presentation</t>
+    <t>Writing Assignment 1: Ouline</t>
   </si>
 </sst>
 </file>
@@ -1607,40 +1607,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>33.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.25</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.25</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.25</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.25</c:v>
+                  <c:v>-4.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.25</c:v>
+                  <c:v>-12.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6.75</c:v>
+                  <c:v>-20.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-14.75</c:v>
+                  <c:v>-28.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22.75</c:v>
+                  <c:v>-36.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-22.75</c:v>
+                  <c:v>-36.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-30.75</c:v>
+                  <c:v>-44.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-38.75</c:v>
+                  <c:v>-52.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1757,40 +1757,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2384,7 +2384,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2538,14 +2538,14 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="19">
         <v>2</v>
       </c>
       <c r="D4" s="12">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="13">
         <f t="shared" si="1"/>
@@ -2581,20 +2581,20 @@
     </row>
     <row r="6" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="22"/>
@@ -2609,14 +2609,14 @@
         <v>20</v>
       </c>
       <c r="C7" s="19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" s="12">
         <v>0</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F7" s="14"/>
       <c r="H7" s="22"/>
@@ -3064,15 +3064,15 @@
       <c r="B35" s="26"/>
       <c r="C35" s="27">
         <f>SUM(C3:C34)</f>
-        <v>33.25</v>
+        <v>19.25</v>
       </c>
       <c r="D35" s="28">
         <f>SUM(D3:D34)</f>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="E35" s="28">
         <f>SUM(E3:E34)</f>
-        <v>33.25</v>
+        <v>19.25</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="30">
@@ -3133,7 +3133,7 @@
       <c r="B36" s="31"/>
       <c r="C36" s="32">
         <f>C35-SUM(G36:W36)</f>
-        <v>-38.75</v>
+        <v>-52.75</v>
       </c>
       <c r="D36" s="33"/>
       <c r="E36" s="34"/>
@@ -3192,51 +3192,51 @@
       </c>
       <c r="F37" s="39">
         <f>C35</f>
-        <v>33.25</v>
+        <v>19.25</v>
       </c>
       <c r="G37" s="41">
         <f t="shared" ref="G37:Q37" si="4">F37-G36</f>
-        <v>33.25</v>
+        <v>19.25</v>
       </c>
       <c r="H37" s="41">
         <f t="shared" si="4"/>
-        <v>25.25</v>
+        <v>11.25</v>
       </c>
       <c r="I37" s="41">
         <f t="shared" si="4"/>
-        <v>17.25</v>
+        <v>3.25</v>
       </c>
       <c r="J37" s="41">
         <f t="shared" si="4"/>
-        <v>9.25</v>
+        <v>-4.75</v>
       </c>
       <c r="K37" s="41">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>-12.75</v>
       </c>
       <c r="L37" s="41">
         <f t="shared" si="4"/>
-        <v>-6.75</v>
+        <v>-20.75</v>
       </c>
       <c r="M37" s="41">
         <f t="shared" si="4"/>
-        <v>-14.75</v>
+        <v>-28.75</v>
       </c>
       <c r="N37" s="41">
         <f t="shared" si="4"/>
-        <v>-22.75</v>
+        <v>-36.75</v>
       </c>
       <c r="O37" s="41">
         <f t="shared" si="4"/>
-        <v>-22.75</v>
+        <v>-36.75</v>
       </c>
       <c r="P37" s="41">
         <f t="shared" si="4"/>
-        <v>-30.75</v>
+        <v>-44.75</v>
       </c>
       <c r="Q37" s="41">
         <f t="shared" si="4"/>
-        <v>-38.75</v>
+        <v>-52.75</v>
       </c>
       <c r="R37" s="41"/>
       <c r="S37" s="42"/>
@@ -3259,51 +3259,51 @@
       </c>
       <c r="F38" s="39">
         <f>D35</f>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="G38" s="39">
         <f>$D$35-SUM(G$3:G$34)</f>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="H38" s="39">
         <f t="shared" ref="H38:Q38" si="5">G38-SUM(H3:H34)</f>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="I38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="J38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="K38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="L38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="M38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="N38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="O38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="P38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="Q38" s="39">
         <f t="shared" si="5"/>
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="R38" s="39"/>
       <c r="S38" s="39"/>
@@ -3979,7 +3979,7 @@
     <row r="6" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>IF(ISBLANK(Chart!A6),"",Chart!A6)</f>
-        <v>Writing Assignment 1: Proposal</v>
+        <v>Writing Assignment 1: Ouline</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(ISBLANK(Chart!B6),"",Chart!B6)</f>

</xml_diff>